<commit_message>
Added win, lose and reset functionality
</commit_message>
<xml_diff>
--- a/Lab1 Time Tracking.xlsx
+++ b/Lab1 Time Tracking.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\GDS1\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\GDS1\GDS1L1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9693DE02-7FFD-4ABF-8BBD-FF5070384469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED15DE73-6408-42FE-838F-611DE81B79D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7AB62D65-D3E9-4090-8EB2-B011564853B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7AB62D65-D3E9-4090-8EB2-B011564853B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,17 +467,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -499,7 +499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -510,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -521,7 +521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -543,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -565,7 +565,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -576,7 +576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -587,20 +587,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>